<commit_message>
split up in smaller functions
</commit_message>
<xml_diff>
--- a/testing/aimlconverter/DE_Training.xlsx
+++ b/testing/aimlconverter/DE_Training.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\EmeraldAI\testing\aimlconverter\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25860" windowHeight="16660"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="128">
   <si>
     <t>Requirement</t>
   </si>
@@ -375,13 +373,46 @@
   </si>
   <si>
     <t>Ich bin {firstname}{lastname}</t>
+  </si>
+  <si>
+    <t>Wie ist dein aktueller Status?</t>
+  </si>
+  <si>
+    <t>{botstatus}</t>
+  </si>
+  <si>
+    <t>{botbattery}</t>
+  </si>
+  <si>
+    <t>battery status</t>
+  </si>
+  <si>
+    <t>important entry in status log</t>
+  </si>
+  <si>
+    <t>Meine Batterie ist bei {botbattery}.</t>
+  </si>
+  <si>
+    <t>BotStatus:eq1</t>
+  </si>
+  <si>
+    <t>BotStatus:gt1</t>
+  </si>
+  <si>
+    <t>Meine Batterie ist bei {botbattery}. Folgende Einträge stind im Status Log: {botstatus}</t>
+  </si>
+  <si>
+    <t>Meine Batterie ist bei {botbattery}. Folgender Eintrag ist im Status Log: {botstatus}</t>
+  </si>
+  <si>
+    <t>BotStatus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,6 +424,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -415,227 +462,45 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="15">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <fill>
         <patternFill>
@@ -804,7 +669,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -839,7 +704,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1016,7 +881,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1024,28 +889,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" customWidth="1"/>
-    <col min="3" max="3" width="67.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" customWidth="1"/>
+    <col min="2" max="2" width="30.5" customWidth="1"/>
+    <col min="3" max="3" width="67.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="B2" t="s">
         <v>77</v>
       </c>
@@ -1053,7 +918,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="B4" t="s">
         <v>53</v>
       </c>
@@ -1061,27 +926,27 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="C5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="C6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="C7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="B10" t="s">
         <v>59</v>
       </c>
@@ -1095,7 +960,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="B11" t="s">
         <v>60</v>
       </c>
@@ -1109,7 +974,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="B12" t="s">
         <v>61</v>
       </c>
@@ -1123,7 +988,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="B13" t="s">
         <v>62</v>
       </c>
@@ -1137,7 +1002,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="B14" t="s">
         <v>63</v>
       </c>
@@ -1145,12 +1010,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="B17" t="s">
         <v>70</v>
       </c>
@@ -1158,7 +1023,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="B18" t="s">
         <v>72</v>
       </c>
@@ -1166,7 +1031,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="B19" t="s">
         <v>86</v>
       </c>
@@ -1174,224 +1039,212 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="20" spans="1:6">
+      <c r="B20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="B21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" t="s">
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
         <v>6</v>
       </c>
-      <c r="E22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
         <v>12</v>
       </c>
-      <c r="E23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
         <v>22</v>
       </c>
-      <c r="E24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
         <v>23</v>
       </c>
-      <c r="E25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
         <v>24</v>
       </c>
-      <c r="E26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
         <v>25</v>
       </c>
-      <c r="E27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
         <v>26</v>
       </c>
-      <c r="E28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
         <v>27</v>
       </c>
-      <c r="E29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
         <v>29</v>
       </c>
-      <c r="D30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
         <v>28</v>
       </c>
-      <c r="D31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
         <v>30</v>
       </c>
-      <c r="D32" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" t="s">
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" t="s">
         <v>31</v>
       </c>
-      <c r="D33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" t="s">
         <v>74</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C36" t="s">
         <v>75</v>
       </c>
-      <c r="D34" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>8</v>
-      </c>
-      <c r="B35" t="s">
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
         <v>79</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C37" t="s">
         <v>80</v>
       </c>
-      <c r="D35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" t="s">
-        <v>15</v>
-      </c>
-      <c r="D37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -1399,16 +1252,13 @@
         <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D38" t="s">
         <v>7</v>
       </c>
-      <c r="E38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -1416,24 +1266,21 @@
         <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D39" t="s">
         <v>7</v>
       </c>
-      <c r="E39" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
@@ -1442,15 +1289,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C41" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D41" t="s">
         <v>7</v>
@@ -1459,15 +1306,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D42" t="s">
         <v>7</v>
@@ -1476,411 +1323,411 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>8</v>
       </c>
       <c r="B43" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
         <v>9</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" t="s">
         <v>11</v>
       </c>
-      <c r="D43" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
         <v>33</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E47" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" t="s">
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
         <v>35</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D48" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>8</v>
-      </c>
-      <c r="B47" t="s">
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" t="s">
         <v>36</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C49" t="s">
         <v>34</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D49" t="s">
         <v>37</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E49" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" t="s">
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
         <v>38</v>
-      </c>
-      <c r="E49" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" t="s">
-        <v>37</v>
-      </c>
-      <c r="E50" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" t="s">
-        <v>81</v>
       </c>
       <c r="E51" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E52" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="E53" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C54" t="s">
+        <v>39</v>
+      </c>
+      <c r="E54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>40</v>
+      </c>
+      <c r="E55" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" t="s">
         <v>43</v>
-      </c>
-      <c r="D54" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" t="s">
-        <v>42</v>
-      </c>
-      <c r="D55" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>8</v>
-      </c>
-      <c r="B56" t="s">
-        <v>44</v>
-      </c>
-      <c r="C56" t="s">
-        <v>41</v>
       </c>
       <c r="D56" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" t="s">
+        <v>42</v>
+      </c>
+      <c r="D57" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="B58" t="s">
+        <v>44</v>
       </c>
       <c r="C58" t="s">
+        <v>41</v>
+      </c>
+      <c r="D58" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
         <v>45</v>
-      </c>
-      <c r="E58" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" t="s">
-        <v>46</v>
-      </c>
-      <c r="E59" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" t="s">
-        <v>47</v>
       </c>
       <c r="E60" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="E61" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>48</v>
-      </c>
-      <c r="D62" t="s">
+        <v>47</v>
+      </c>
+      <c r="E62" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>8</v>
-      </c>
-      <c r="B63" t="s">
-        <v>74</v>
+        <v>5</v>
       </c>
       <c r="C63" t="s">
-        <v>49</v>
-      </c>
-      <c r="D63" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="E63" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" t="s">
+        <v>48</v>
+      </c>
+      <c r="D64" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="B65" t="s">
+        <v>74</v>
       </c>
       <c r="C65" t="s">
+        <v>49</v>
+      </c>
+      <c r="D65" t="s">
+        <v>51</v>
+      </c>
+      <c r="E65" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" t="s">
         <v>82</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E67" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>5</v>
-      </c>
-      <c r="C66" t="s">
+    <row r="68" spans="1:6">
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" t="s">
         <v>83</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E68" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>8</v>
-      </c>
-      <c r="C67" t="s">
+    <row r="69" spans="1:6">
+      <c r="A69" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" t="s">
         <v>85</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D69" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" t="s">
+    <row r="71" spans="1:6">
+      <c r="A71" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>8</v>
-      </c>
-      <c r="B70" t="s">
+    <row r="72" spans="1:6">
+      <c r="A72" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" t="s">
         <v>97</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C72" t="s">
         <v>98</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F72" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>8</v>
-      </c>
-      <c r="B71" t="s">
+    <row r="73" spans="1:6">
+      <c r="A73" t="s">
+        <v>8</v>
+      </c>
+      <c r="B73" t="s">
         <v>97</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C73" t="s">
         <v>99</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F73" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" t="s">
+    <row r="75" spans="1:6">
+      <c r="A75" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" t="s">
         <v>115</v>
-      </c>
-      <c r="E73" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>5</v>
-      </c>
-      <c r="C74" t="s">
-        <v>114</v>
-      </c>
-      <c r="E74" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" t="s">
-        <v>113</v>
       </c>
       <c r="E75" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
         <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E76" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
         <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E77" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
         <v>5</v>
       </c>
       <c r="C78" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E78" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
         <v>5</v>
       </c>
       <c r="C79" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E79" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>8</v>
-      </c>
-      <c r="B80" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" t="s">
+        <v>110</v>
+      </c>
+      <c r="E80" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" t="s">
+        <v>111</v>
+      </c>
+      <c r="E81" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82" t="s">
         <v>100</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C82" t="s">
         <v>105</v>
-      </c>
-      <c r="D80" t="s">
-        <v>112</v>
-      </c>
-      <c r="F80" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>8</v>
-      </c>
-      <c r="B81" t="s">
-        <v>101</v>
-      </c>
-      <c r="C81" t="s">
-        <v>107</v>
-      </c>
-      <c r="D81" t="s">
-        <v>112</v>
-      </c>
-      <c r="F81" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>8</v>
-      </c>
-      <c r="B82" t="s">
-        <v>102</v>
-      </c>
-      <c r="C82" t="s">
-        <v>106</v>
       </c>
       <c r="D82" t="s">
         <v>112</v>
@@ -1889,32 +1736,132 @@
         <v>104</v>
       </c>
     </row>
+    <row r="83" spans="1:6">
+      <c r="A83" t="s">
+        <v>8</v>
+      </c>
+      <c r="B83" t="s">
+        <v>101</v>
+      </c>
+      <c r="C83" t="s">
+        <v>107</v>
+      </c>
+      <c r="D83" t="s">
+        <v>112</v>
+      </c>
+      <c r="F83" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" t="s">
+        <v>8</v>
+      </c>
+      <c r="B84" t="s">
+        <v>102</v>
+      </c>
+      <c r="C84" t="s">
+        <v>106</v>
+      </c>
+      <c r="D84" t="s">
+        <v>112</v>
+      </c>
+      <c r="F84" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" t="s">
+        <v>54</v>
+      </c>
+      <c r="E86" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" t="s">
+        <v>117</v>
+      </c>
+      <c r="E87" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" t="s">
+        <v>122</v>
+      </c>
+      <c r="D88" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" t="s">
+        <v>8</v>
+      </c>
+      <c r="B89" t="s">
+        <v>123</v>
+      </c>
+      <c r="C89" t="s">
+        <v>126</v>
+      </c>
+      <c r="D89" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90" t="s">
+        <v>124</v>
+      </c>
+      <c r="C90" t="s">
+        <v>125</v>
+      </c>
+      <c r="D90" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A34:E34 A73:F502">
-    <cfRule type="expression" dxfId="9" priority="3">
-      <formula>$A34="A"</formula>
+  <conditionalFormatting sqref="A36:E36 A75:F504">
+    <cfRule type="expression" dxfId="15" priority="3">
+      <formula>$A36="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="4">
-      <formula>$A34="Q"</formula>
+    <cfRule type="expression" dxfId="14" priority="4">
+      <formula>$A36="Q"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A50:E50">
-    <cfRule type="expression" dxfId="7" priority="1">
-      <formula>$A50="A"</formula>
+  <conditionalFormatting sqref="A52:E52">
+    <cfRule type="expression" dxfId="13" priority="1">
+      <formula>$A52="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
-      <formula>$A50="Q"</formula>
+    <cfRule type="expression" dxfId="12" priority="2">
+      <formula>$A52="Q"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A22:F72">
-    <cfRule type="expression" dxfId="5" priority="5">
-      <formula>$A22="A"</formula>
+  <conditionalFormatting sqref="A24:F74">
+    <cfRule type="expression" dxfId="11" priority="5">
+      <formula>$A24="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
-      <formula>$A22="Q"</formula>
+    <cfRule type="expression" dxfId="10" priority="6">
+      <formula>$A24="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Combine Conversation classes - Dialog and Command
</commit_message>
<xml_diff>
--- a/testing/aimlconverter/DE_Training.xlsx
+++ b/testing/aimlconverter/DE_Training.xlsx
@@ -348,9 +348,6 @@
     <t>Hallo {nametitle}{fullname}</t>
   </si>
   <si>
-    <t>Follow Up Action</t>
-  </si>
-  <si>
     <t>{firstname}</t>
   </si>
   <si>
@@ -406,6 +403,9 @@
   </si>
   <si>
     <t>UserType:Admin|BotStatus:gt1</t>
+  </si>
+  <si>
+    <t>Action</t>
   </si>
 </sst>
 </file>
@@ -1035,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1185,18 +1185,18 @@
     </row>
     <row r="20" spans="1:6">
       <c r="B20" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" t="s">
         <v>119</v>
-      </c>
-      <c r="C20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="B21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1216,7 +1216,7 @@
         <v>3</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1464,7 +1464,7 @@
         <v>7</v>
       </c>
       <c r="E42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1481,7 +1481,7 @@
         <v>7</v>
       </c>
       <c r="E43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1791,10 +1791,10 @@
         <v>5</v>
       </c>
       <c r="C75" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E75" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -1802,10 +1802,10 @@
         <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E76" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -1813,10 +1813,10 @@
         <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E77" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -1824,10 +1824,10 @@
         <v>5</v>
       </c>
       <c r="C78" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E78" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -1835,10 +1835,10 @@
         <v>5</v>
       </c>
       <c r="C79" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E79" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -1846,10 +1846,10 @@
         <v>5</v>
       </c>
       <c r="C80" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E80" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -1857,10 +1857,10 @@
         <v>5</v>
       </c>
       <c r="C81" t="s">
+        <v>110</v>
+      </c>
+      <c r="E81" t="s">
         <v>111</v>
-      </c>
-      <c r="E81" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -1874,7 +1874,7 @@
         <v>105</v>
       </c>
       <c r="D82" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F82" t="s">
         <v>104</v>
@@ -1891,7 +1891,7 @@
         <v>107</v>
       </c>
       <c r="D83" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F83" t="s">
         <v>104</v>
@@ -1908,7 +1908,7 @@
         <v>106</v>
       </c>
       <c r="D84" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F84" t="s">
         <v>104</v>
@@ -1930,7 +1930,7 @@
         <v>5</v>
       </c>
       <c r="C87" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E87" t="s">
         <v>21</v>
@@ -1941,7 +1941,7 @@
         <v>8</v>
       </c>
       <c r="C88" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D88" t="s">
         <v>21</v>
@@ -1952,10 +1952,10 @@
         <v>8</v>
       </c>
       <c r="B89" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C89" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D89" t="s">
         <v>21</v>
@@ -1966,10 +1966,10 @@
         <v>8</v>
       </c>
       <c r="B90" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C90" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D90" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Extend Excel training file
</commit_message>
<xml_diff>
--- a/testing/aimlconverter/DE_Training.xlsx
+++ b/testing/aimlconverter/DE_Training.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="197">
   <si>
     <t>Requirement</t>
   </si>
@@ -500,9 +500,6 @@
     <t>Liebevolle Wörter: Ich mag dich</t>
   </si>
   <si>
-    <t>Beleidigungen</t>
-  </si>
-  <si>
     <t>Machs gut</t>
   </si>
   <si>
@@ -512,9 +509,6 @@
     <t>Bist du ein Robotter</t>
   </si>
   <si>
-    <t>Wer hat dich gebaut</t>
-  </si>
-  <si>
     <t>Bist du ein Junde oder ein Mädchen</t>
   </si>
   <si>
@@ -527,31 +521,103 @@
     <t>Wie geht’s dir?</t>
   </si>
   <si>
-    <t>Wie alt bist du</t>
-  </si>
-  <si>
-    <t>Wo lebst du</t>
-  </si>
-  <si>
-    <t>wo wohnst du</t>
-  </si>
-  <si>
-    <t>wo kommst du her</t>
-  </si>
-  <si>
-    <t>Wieviel uhr ist es</t>
-  </si>
-  <si>
-    <t>wie spät ist es</t>
-  </si>
-  <si>
-    <t>wieviel uhr haben wir</t>
-  </si>
-  <si>
-    <t>was magst du</t>
-  </si>
-  <si>
-    <t>was sind eeine hobbies</t>
+    <t>Was magst du?</t>
+  </si>
+  <si>
+    <t>Was sind deine Hobbies?</t>
+  </si>
+  <si>
+    <t>Smalltalk</t>
+  </si>
+  <si>
+    <t>Ich bin noch nicht so weit Entwickelt eigene Vorlieben oder Hobbies zu haben.</t>
+  </si>
+  <si>
+    <t>Wieviel Uhr ist es?</t>
+  </si>
+  <si>
+    <t>Wie spät ist es?</t>
+  </si>
+  <si>
+    <t>Wieviel Uhr haben wir?</t>
+  </si>
+  <si>
+    <t>Welcher Tag ist heute?</t>
+  </si>
+  <si>
+    <t>Der wievielite ist heute?</t>
+  </si>
+  <si>
+    <t>Den wievielten haben wir?</t>
+  </si>
+  <si>
+    <t>Heute ist {weekday} der {date}</t>
+  </si>
+  <si>
+    <t>Es ist gerade {time}Uhr</t>
+  </si>
+  <si>
+    <t>Wir haben gerade {time}Uhr</t>
+  </si>
+  <si>
+    <t>Wir haben heute {weekday} den {date}</t>
+  </si>
+  <si>
+    <t>Wo lebst du?</t>
+  </si>
+  <si>
+    <t>Wo wohnst du?</t>
+  </si>
+  <si>
+    <t>Wo Kommst du her?</t>
+  </si>
+  <si>
+    <t>Wo wurdest du entwickelt?</t>
+  </si>
+  <si>
+    <t>Ich bin eine Maschine. Ich lebe dort wo man mich plaziert.</t>
+  </si>
+  <si>
+    <t>Ich bin nicht darauf Programmiert eigenen Aktivitäten nachzugehen.</t>
+  </si>
+  <si>
+    <t>Ich habe keinen Wohnort im herkömmluchen Sinne.</t>
+  </si>
+  <si>
+    <t>Ich wurde in {botorigin} entwickelt.</t>
+  </si>
+  <si>
+    <t>Mein Entwickler kommt aus {botorigin}.</t>
+  </si>
+  <si>
+    <t>Wie alt bist du?</t>
+  </si>
+  <si>
+    <t>Wann bist du geboren?</t>
+  </si>
+  <si>
+    <t>Ich bin seit dem {botbuilddate} in Entwicklung.</t>
+  </si>
+  <si>
+    <t>Meine erste Zeile Code wurde am {botbuilddate} geschrieben.</t>
+  </si>
+  <si>
+    <t>Wer sind deine Erbauer?</t>
+  </si>
+  <si>
+    <t>Wer hat dich gebaut?</t>
+  </si>
+  <si>
+    <t>Wer hat dich Programmiert?</t>
+  </si>
+  <si>
+    <t>Ich wurde von {botdeveloper} entwickelt.</t>
+  </si>
+  <si>
+    <t>Hauptsächlich wurde ich von {botdeveloper} programmiert.</t>
+  </si>
+  <si>
+    <t>Joke</t>
   </si>
 </sst>
 </file>
@@ -650,7 +716,1127 @@
     <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="204">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1235,17 +2421,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F151"/>
+  <dimension ref="A1:F173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="C151" sqref="C151"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" customWidth="1"/>
     <col min="2" max="2" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
@@ -1570,7 +2756,7 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E40" t="s">
         <v>7</v>
@@ -1883,7 +3069,7 @@
         <v>5</v>
       </c>
       <c r="C65" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E65" t="s">
         <v>37</v>
@@ -2210,7 +3396,7 @@
         <v>5</v>
       </c>
       <c r="C97" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E97" t="s">
         <v>21</v>
@@ -2344,6 +3530,11 @@
       </c>
       <c r="F109" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="114" spans="3:3" x14ac:dyDescent="0.25">
@@ -2383,12 +3574,12 @@
     </row>
     <row r="123" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C123" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="124" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C124" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="125" spans="3:3" x14ac:dyDescent="0.25">
@@ -2398,7 +3589,7 @@
     </row>
     <row r="126" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C126" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="127" spans="3:3" x14ac:dyDescent="0.25">
@@ -2408,214 +3599,401 @@
     </row>
     <row r="128" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C128" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>5</v>
+      </c>
       <c r="C130" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E130" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>5</v>
+      </c>
       <c r="C131" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C133" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C135" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E131" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>8</v>
+      </c>
+      <c r="C132" t="s">
+        <v>142</v>
+      </c>
+      <c r="D132" t="s">
+        <v>166</v>
+      </c>
+      <c r="F132" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>5</v>
+      </c>
+      <c r="C137" t="s">
+        <v>192</v>
+      </c>
+      <c r="E137" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>5</v>
+      </c>
       <c r="C138" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="E138" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>5</v>
+      </c>
+      <c r="C139" t="s">
+        <v>193</v>
+      </c>
+      <c r="E139" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>8</v>
+      </c>
       <c r="C140" t="s">
+        <v>194</v>
+      </c>
+      <c r="D140" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C142" t="s">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>8</v>
+      </c>
+      <c r="C141" t="s">
+        <v>195</v>
+      </c>
+      <c r="D141" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>5</v>
+      </c>
+      <c r="C143" t="s">
+        <v>187</v>
+      </c>
+      <c r="E143" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>5</v>
+      </c>
+      <c r="C144" t="s">
+        <v>188</v>
+      </c>
+      <c r="E144" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>8</v>
+      </c>
+      <c r="C145" t="s">
+        <v>189</v>
+      </c>
+      <c r="D145" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>8</v>
+      </c>
+      <c r="C146" t="s">
+        <v>190</v>
+      </c>
+      <c r="D146" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>5</v>
+      </c>
+      <c r="C148" t="s">
+        <v>178</v>
+      </c>
+      <c r="E148" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>5</v>
+      </c>
+      <c r="C149" t="s">
+        <v>179</v>
+      </c>
+      <c r="E149" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>8</v>
+      </c>
+      <c r="C150" t="s">
+        <v>182</v>
+      </c>
+      <c r="D150" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>8</v>
+      </c>
+      <c r="C151" t="s">
+        <v>184</v>
+      </c>
+      <c r="D151" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>5</v>
+      </c>
+      <c r="C153" t="s">
+        <v>180</v>
+      </c>
+      <c r="E153" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>5</v>
+      </c>
+      <c r="C154" t="s">
+        <v>181</v>
+      </c>
+      <c r="E154" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>8</v>
+      </c>
+      <c r="C155" t="s">
+        <v>185</v>
+      </c>
+      <c r="D155" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>8</v>
+      </c>
+      <c r="C156" t="s">
+        <v>186</v>
+      </c>
+      <c r="D156" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>5</v>
+      </c>
+      <c r="C158" t="s">
+        <v>168</v>
+      </c>
+      <c r="E158" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>5</v>
+      </c>
+      <c r="C159" t="s">
+        <v>169</v>
+      </c>
+      <c r="E159" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>5</v>
+      </c>
+      <c r="C160" t="s">
+        <v>170</v>
+      </c>
+      <c r="E160" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>8</v>
+      </c>
+      <c r="C161" t="s">
+        <v>175</v>
+      </c>
+      <c r="D161" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>8</v>
+      </c>
+      <c r="C162" t="s">
+        <v>176</v>
+      </c>
+      <c r="D162" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>5</v>
+      </c>
+      <c r="C164" t="s">
+        <v>171</v>
+      </c>
+      <c r="E164" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>5</v>
+      </c>
+      <c r="C165" t="s">
+        <v>172</v>
+      </c>
+      <c r="E165" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>5</v>
+      </c>
+      <c r="C166" t="s">
+        <v>173</v>
+      </c>
+      <c r="E166" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>8</v>
+      </c>
+      <c r="C167" t="s">
+        <v>174</v>
+      </c>
+      <c r="D167" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>8</v>
+      </c>
+      <c r="C168" t="s">
+        <v>177</v>
+      </c>
+      <c r="D168" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>5</v>
+      </c>
+      <c r="C170" t="s">
+        <v>164</v>
+      </c>
+      <c r="E170" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>5</v>
+      </c>
+      <c r="C171" t="s">
+        <v>165</v>
+      </c>
+      <c r="E171" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>8</v>
+      </c>
+      <c r="C172" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C143" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C144" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C146" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C147" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C148" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="150" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C150" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="151" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C151" t="s">
-        <v>174</v>
+      <c r="D172" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>8</v>
+      </c>
+      <c r="C173" t="s">
+        <v>183</v>
+      </c>
+      <c r="D173" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A45:E45 A85:F95 A98:D99 F98:F99 A100:C102 E100:F102 A103:F122 A127:F519 A125:F125">
-    <cfRule type="expression" dxfId="37" priority="31">
-      <formula>$A45="A"</formula>
+  <conditionalFormatting sqref="A1:F111 A112:B112 D112:F112 A113:F1048576">
+    <cfRule type="expression" dxfId="3" priority="61">
+      <formula>$A1="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="32">
-      <formula>$A45="Q"</formula>
+    <cfRule type="expression" dxfId="2" priority="62">
+      <formula>$A1="Q"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A61:E61">
-    <cfRule type="expression" dxfId="35" priority="29">
-      <formula>$A61="A"</formula>
+  <conditionalFormatting sqref="C112">
+    <cfRule type="expression" dxfId="1" priority="71">
+      <formula>#REF!="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="30">
-      <formula>$A61="Q"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31:F37 A40:F64 A66:F84">
-    <cfRule type="expression" dxfId="33" priority="33">
-      <formula>$A31="A"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="34">
-      <formula>$A31="Q"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E98">
-    <cfRule type="expression" dxfId="31" priority="27">
-      <formula>$A98="A"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="28">
-      <formula>$A98="Q"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E99">
-    <cfRule type="expression" dxfId="29" priority="25">
-      <formula>$A99="A"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="26">
-      <formula>$A99="Q"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D100">
-    <cfRule type="expression" dxfId="27" priority="23">
-      <formula>$A100="A"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="24">
-      <formula>$A100="Q"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D101">
-    <cfRule type="expression" dxfId="25" priority="21">
-      <formula>$A101="A"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="22">
-      <formula>$A101="Q"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D102">
-    <cfRule type="expression" dxfId="23" priority="19">
-      <formula>$A102="A"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="20">
-      <formula>$A102="Q"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38:F38">
-    <cfRule type="expression" dxfId="21" priority="17">
-      <formula>$A38="A"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="18">
-      <formula>$A38="Q"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A97:D97 F97">
-    <cfRule type="expression" dxfId="19" priority="15">
-      <formula>$A97="A"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="16">
-      <formula>$A97="Q"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E97">
-    <cfRule type="expression" dxfId="17" priority="13">
-      <formula>$A97="A"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="14">
-      <formula>$A97="Q"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65:F65">
-    <cfRule type="expression" dxfId="15" priority="11">
-      <formula>$A65="A"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="12">
-      <formula>$A65="Q"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A39:F39">
-    <cfRule type="expression" dxfId="13" priority="9">
-      <formula>$A39="A"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="10">
-      <formula>$A39="Q"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A126:F126">
-    <cfRule type="expression" dxfId="11" priority="7">
-      <formula>$A126="A"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="8">
-      <formula>$A126="Q"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A123:F124">
-    <cfRule type="expression" dxfId="9" priority="5">
-      <formula>$A123="A"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6">
-      <formula>$A123="Q"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A96:D96 F96">
-    <cfRule type="expression" dxfId="7" priority="3">
-      <formula>$A96="A"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4">
-      <formula>$A96="Q"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E96">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$A96="A"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$A96="Q"</formula>
+    <cfRule type="expression" dxfId="0" priority="72">
+      <formula>#REF!="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
extend training file and add excel to csv test
</commit_message>
<xml_diff>
--- a/testing/aimlconverter/DE_Training.xlsx
+++ b/testing/aimlconverter/DE_Training.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\EmeraldAI\testing\aimlconverter\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25860" windowHeight="16660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25860" windowHeight="16665"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="209">
   <si>
     <t>Requirement</t>
   </si>
@@ -625,6 +630,30 @@
   </si>
   <si>
     <t>Wie kann ich Ihnen behilflich sein?</t>
+  </si>
+  <si>
+    <t>TRIGGER_FACEAPP_ON</t>
+  </si>
+  <si>
+    <t>TRIGGER_FACEAPP_OFF</t>
+  </si>
+  <si>
+    <t>TRIGGER</t>
+  </si>
+  <si>
+    <t>Hey, wer hat das List aus gemacht?</t>
+  </si>
+  <si>
+    <t>{name} warum haben Sie mein Display deaktiviert?</t>
+  </si>
+  <si>
+    <t>Das ist aber nicht nett {name}. Machen Sie bitte mein Display wieder an.</t>
+  </si>
+  <si>
+    <t>Danke, dass Sie mein Display wieder eingeschatet haben.</t>
+  </si>
+  <si>
+    <t>Danke! Sehr nett von Ihnen.</t>
   </si>
 </sst>
 </file>
@@ -707,15 +736,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -727,7 +756,133 @@
     <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="22">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1024,7 +1179,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1032,28 +1187,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F169"/>
+  <dimension ref="A1:F179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="C123" sqref="C123"/>
+    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="C175" sqref="C175"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" customWidth="1"/>
-    <col min="2" max="2" width="39.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="77.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>77</v>
       </c>
@@ -1061,7 +1216,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>53</v>
       </c>
@@ -1069,27 +1224,27 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>59</v>
       </c>
@@ -1103,7 +1258,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>60</v>
       </c>
@@ -1117,7 +1272,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>61</v>
       </c>
@@ -1131,7 +1286,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>62</v>
       </c>
@@ -1145,7 +1300,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>63</v>
       </c>
@@ -1153,12 +1308,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>70</v>
       </c>
@@ -1166,7 +1321,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>72</v>
       </c>
@@ -1174,7 +1329,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>86</v>
       </c>
@@ -1182,7 +1337,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>113</v>
       </c>
@@ -1190,7 +1345,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>112</v>
       </c>
@@ -1198,12 +1353,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>123</v>
       </c>
@@ -1211,7 +1366,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>125</v>
       </c>
@@ -1219,7 +1374,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>127</v>
       </c>
@@ -1227,7 +1382,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>129</v>
       </c>
@@ -1235,7 +1390,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>131</v>
       </c>
@@ -1243,7 +1398,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>4</v>
       </c>
@@ -1263,7 +1418,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -1274,7 +1429,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -1285,7 +1440,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -1296,7 +1451,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1307,7 +1462,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1318,7 +1473,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1329,7 +1484,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -1340,7 +1495,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1351,7 +1506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -1362,7 +1517,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -1373,7 +1528,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -1384,7 +1539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -1395,7 +1550,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -1409,7 +1564,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>8</v>
       </c>
@@ -1420,7 +1575,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -1437,7 +1592,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -1454,7 +1609,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -1468,7 +1623,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -1482,7 +1637,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -1499,7 +1654,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -1516,7 +1671,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -1533,7 +1688,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -1550,7 +1705,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -1567,7 +1722,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -1581,7 +1736,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>5</v>
       </c>
@@ -1592,7 +1747,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>8</v>
       </c>
@@ -1603,7 +1758,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>8</v>
       </c>
@@ -1620,7 +1775,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>5</v>
       </c>
@@ -1631,7 +1786,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -1642,7 +1797,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>5</v>
       </c>
@@ -1653,7 +1808,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>5</v>
       </c>
@@ -1664,7 +1819,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>5</v>
       </c>
@@ -1675,7 +1830,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -1686,7 +1841,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -1697,7 +1852,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -1708,7 +1863,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -1722,7 +1877,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>5</v>
       </c>
@@ -1733,7 +1888,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>5</v>
       </c>
@@ -1744,7 +1899,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>5</v>
       </c>
@@ -1755,7 +1910,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>5</v>
       </c>
@@ -1766,7 +1921,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -1777,7 +1932,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>8</v>
       </c>
@@ -1794,7 +1949,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>5</v>
       </c>
@@ -1805,7 +1960,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>5</v>
       </c>
@@ -1816,7 +1971,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -1827,7 +1982,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>5</v>
       </c>
@@ -1835,7 +1990,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>8</v>
       </c>
@@ -1849,7 +2004,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>8</v>
       </c>
@@ -1863,7 +2018,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>5</v>
       </c>
@@ -1874,7 +2029,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>5</v>
       </c>
@@ -1885,7 +2040,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>5</v>
       </c>
@@ -1896,7 +2051,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>5</v>
       </c>
@@ -1907,7 +2062,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>5</v>
       </c>
@@ -1918,7 +2073,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>5</v>
       </c>
@@ -1929,7 +2084,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>5</v>
       </c>
@@ -1940,7 +2095,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>8</v>
       </c>
@@ -1957,7 +2112,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>8</v>
       </c>
@@ -1974,7 +2129,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>8</v>
       </c>
@@ -1991,7 +2146,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>5</v>
       </c>
@@ -2002,7 +2157,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>5</v>
       </c>
@@ -2013,7 +2168,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>5</v>
       </c>
@@ -2024,7 +2179,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>5</v>
       </c>
@@ -2035,7 +2190,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>8</v>
       </c>
@@ -2046,7 +2201,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>8</v>
       </c>
@@ -2060,7 +2215,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>8</v>
       </c>
@@ -2074,7 +2229,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>5</v>
       </c>
@@ -2085,7 +2240,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>5</v>
       </c>
@@ -2096,7 +2251,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>5</v>
       </c>
@@ -2107,7 +2262,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>5</v>
       </c>
@@ -2118,7 +2273,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>5</v>
       </c>
@@ -2129,7 +2284,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>8</v>
       </c>
@@ -2143,7 +2298,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>5</v>
       </c>
@@ -2154,7 +2309,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>5</v>
       </c>
@@ -2165,7 +2320,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>5</v>
       </c>
@@ -2176,7 +2331,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>8</v>
       </c>
@@ -2187,7 +2342,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>8</v>
       </c>
@@ -2198,7 +2353,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>8</v>
       </c>
@@ -2209,57 +2364,57 @@
         <v>198</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C118" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C119" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C120" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C121" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C122" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C123" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C124" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C125" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C126" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C127" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>5</v>
       </c>
@@ -2270,7 +2425,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>5</v>
       </c>
@@ -2281,7 +2436,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>8</v>
       </c>
@@ -2295,7 +2450,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>5</v>
       </c>
@@ -2306,7 +2461,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>5</v>
       </c>
@@ -2317,7 +2472,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>5</v>
       </c>
@@ -2328,7 +2483,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>8</v>
       </c>
@@ -2339,7 +2494,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>8</v>
       </c>
@@ -2350,7 +2505,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>5</v>
       </c>
@@ -2361,7 +2516,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>5</v>
       </c>
@@ -2372,7 +2527,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>8</v>
       </c>
@@ -2383,7 +2538,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>8</v>
       </c>
@@ -2394,7 +2549,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>5</v>
       </c>
@@ -2405,7 +2560,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>5</v>
       </c>
@@ -2416,7 +2571,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>8</v>
       </c>
@@ -2427,7 +2582,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>8</v>
       </c>
@@ -2438,7 +2593,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>5</v>
       </c>
@@ -2449,7 +2604,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>5</v>
       </c>
@@ -2460,7 +2615,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="151" spans="1:5">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>8</v>
       </c>
@@ -2471,7 +2626,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="152" spans="1:5">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>8</v>
       </c>
@@ -2482,7 +2637,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="154" spans="1:5">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>5</v>
       </c>
@@ -2493,7 +2648,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>5</v>
       </c>
@@ -2504,7 +2659,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>5</v>
       </c>
@@ -2515,7 +2670,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="157" spans="1:5">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>8</v>
       </c>
@@ -2526,7 +2681,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>8</v>
       </c>
@@ -2537,7 +2692,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>5</v>
       </c>
@@ -2548,7 +2703,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="161" spans="1:5">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>5</v>
       </c>
@@ -2559,7 +2714,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>5</v>
       </c>
@@ -2570,7 +2725,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="163" spans="1:5">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>8</v>
       </c>
@@ -2581,7 +2736,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="164" spans="1:5">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>8</v>
       </c>
@@ -2592,7 +2747,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="166" spans="1:5">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>5</v>
       </c>
@@ -2603,7 +2758,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:5">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>5</v>
       </c>
@@ -2614,7 +2769,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="168" spans="1:5">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>8</v>
       </c>
@@ -2625,7 +2780,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="169" spans="1:5">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>8</v>
       </c>
@@ -2636,20 +2791,100 @@
         <v>165</v>
       </c>
     </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>5</v>
+      </c>
+      <c r="C172" t="s">
+        <v>201</v>
+      </c>
+      <c r="E172" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>8</v>
+      </c>
+      <c r="C173" t="s">
+        <v>207</v>
+      </c>
+      <c r="D173" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>8</v>
+      </c>
+      <c r="C174" t="s">
+        <v>208</v>
+      </c>
+      <c r="D174" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>5</v>
+      </c>
+      <c r="C176" t="s">
+        <v>202</v>
+      </c>
+      <c r="E176" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>8</v>
+      </c>
+      <c r="B177" t="s">
+        <v>74</v>
+      </c>
+      <c r="C177" t="s">
+        <v>204</v>
+      </c>
+      <c r="D177" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>8</v>
+      </c>
+      <c r="C178" t="s">
+        <v>205</v>
+      </c>
+      <c r="D178" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>8</v>
+      </c>
+      <c r="C179" t="s">
+        <v>206</v>
+      </c>
+      <c r="D179" t="s">
+        <v>203</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F110 A117:F1048576">
-    <cfRule type="expression" dxfId="3" priority="63">
+    <cfRule type="expression" dxfId="5" priority="63">
       <formula>$A1="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="64">
+    <cfRule type="expression" dxfId="4" priority="64">
       <formula>$A1="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A111:F116">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$A111="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$A111="Q"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>